<commit_message>
Products per capita files
</commit_message>
<xml_diff>
--- a/retail-power-compare/data/products-you-could-buy-per-capita.xlsx
+++ b/retail-power-compare/data/products-you-could-buy-per-capita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Darren/Github clones/data-projects/retail-power-compare/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FE2DBA-3557-E740-A5F4-78BE9A34E04B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692AE4EE-852F-A94B-B3DB-56FFEE70F5DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{94BEB61A-99A7-6A43-8114-75E7C06F76BC}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="182" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>